<commit_message>
Updated Data dictionary for master db changes which are recently updated
</commit_message>
<xml_diff>
--- a/design/data_model/mosip_master_dd.xlsx
+++ b/design/data_model/mosip_master_dd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045015\git\commons\design\data_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{183F8A4C-74EF-4B3C-98DE-1779910F7D56}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E852F2C7-37CF-4E15-8A58-57C065938A07}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12159" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12986" uniqueCount="731">
   <si>
     <t>app_id</t>
   </si>
@@ -2350,7 +2350,38 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2626,10 +2657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C05F018-83F5-4DEE-9D32-5EB34F77EC11}">
-  <dimension ref="B1:J893"/>
+  <dimension ref="B1:J1054"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A1004" workbookViewId="0">
+      <selection activeCell="C1034" sqref="C1034"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -24354,6 +24385,3913 @@
       <c r="I893" s="7"/>
       <c r="J893" s="7"/>
     </row>
+    <row r="894" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B894" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="C894" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="D894" s="5"/>
+      <c r="E894" s="5"/>
+      <c r="F894" s="5"/>
+      <c r="G894" s="5"/>
+      <c r="H894" s="5"/>
+      <c r="I894" s="5"/>
+      <c r="J894" s="5"/>
+    </row>
+    <row r="895" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B895" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="C895" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D895" s="7" t="s">
+        <v>626</v>
+      </c>
+      <c r="E895" s="7">
+        <v>1</v>
+      </c>
+      <c r="F895" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G895" s="7">
+        <v>3</v>
+      </c>
+      <c r="H895" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I895" s="7" t="s">
+        <v>625</v>
+      </c>
+      <c r="J895" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="896" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B896" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="C896" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D896" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="E896" s="7">
+        <v>2</v>
+      </c>
+      <c r="F896" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G896" s="7">
+        <v>36</v>
+      </c>
+      <c r="H896" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I896" s="7"/>
+      <c r="J896" s="7"/>
+    </row>
+    <row r="897" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B897" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="C897" s="7" t="s">
+        <v>628</v>
+      </c>
+      <c r="D897" s="7" t="s">
+        <v>629</v>
+      </c>
+      <c r="E897" s="7">
+        <v>3</v>
+      </c>
+      <c r="F897" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="G897" s="7"/>
+      <c r="H897" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I897" s="7"/>
+      <c r="J897" s="7"/>
+    </row>
+    <row r="898" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B898" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="C898" s="7" t="s">
+        <v>630</v>
+      </c>
+      <c r="D898" s="7" t="s">
+        <v>631</v>
+      </c>
+      <c r="E898" s="7">
+        <v>4</v>
+      </c>
+      <c r="F898" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G898" s="7"/>
+      <c r="H898" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I898" s="7"/>
+      <c r="J898" s="7"/>
+    </row>
+    <row r="899" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B899" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="C899" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D899" s="7" t="s">
+        <v>632</v>
+      </c>
+      <c r="E899" s="7">
+        <v>5</v>
+      </c>
+      <c r="F899" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G899" s="7">
+        <v>3</v>
+      </c>
+      <c r="H899" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I899" s="7" t="s">
+        <v>625</v>
+      </c>
+      <c r="J899" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="900" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B900" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="C900" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D900" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E900" s="7">
+        <v>6</v>
+      </c>
+      <c r="F900" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G900" s="7"/>
+      <c r="H900" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I900" s="7"/>
+      <c r="J900" s="7"/>
+    </row>
+    <row r="901" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B901" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="C901" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D901" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E901" s="7">
+        <v>7</v>
+      </c>
+      <c r="F901" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G901" s="7">
+        <v>256</v>
+      </c>
+      <c r="H901" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I901" s="7"/>
+      <c r="J901" s="7"/>
+    </row>
+    <row r="902" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B902" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="C902" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D902" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E902" s="7">
+        <v>8</v>
+      </c>
+      <c r="F902" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G902" s="7"/>
+      <c r="H902" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I902" s="7"/>
+      <c r="J902" s="7"/>
+    </row>
+    <row r="903" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B903" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="C903" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D903" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E903" s="7">
+        <v>9</v>
+      </c>
+      <c r="F903" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G903" s="7">
+        <v>256</v>
+      </c>
+      <c r="H903" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I903" s="7"/>
+      <c r="J903" s="7"/>
+    </row>
+    <row r="904" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B904" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="C904" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D904" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E904" s="7">
+        <v>10</v>
+      </c>
+      <c r="F904" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G904" s="7"/>
+      <c r="H904" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I904" s="7"/>
+      <c r="J904" s="7"/>
+    </row>
+    <row r="905" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B905" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="C905" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D905" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E905" s="7">
+        <v>11</v>
+      </c>
+      <c r="F905" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G905" s="7"/>
+      <c r="H905" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I905" s="7"/>
+      <c r="J905" s="7"/>
+    </row>
+    <row r="906" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B906" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="C906" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D906" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E906" s="7">
+        <v>12</v>
+      </c>
+      <c r="F906" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G906" s="7"/>
+      <c r="H906" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I906" s="7"/>
+      <c r="J906" s="7"/>
+    </row>
+    <row r="907" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B907" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="C907" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="D907" s="5"/>
+      <c r="E907" s="5"/>
+      <c r="F907" s="5"/>
+      <c r="G907" s="5"/>
+      <c r="H907" s="5"/>
+      <c r="I907" s="5"/>
+      <c r="J907" s="5"/>
+    </row>
+    <row r="908" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B908" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="C908" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D908" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="E908" s="7">
+        <v>1</v>
+      </c>
+      <c r="F908" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G908" s="7">
+        <v>36</v>
+      </c>
+      <c r="H908" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I908" s="7" t="s">
+        <v>633</v>
+      </c>
+      <c r="J908" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="909" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B909" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="C909" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="D909" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="E909" s="7">
+        <v>2</v>
+      </c>
+      <c r="F909" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G909" s="7">
+        <v>128</v>
+      </c>
+      <c r="H909" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I909" s="7"/>
+      <c r="J909" s="7"/>
+    </row>
+    <row r="910" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B910" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="C910" s="7" t="s">
+        <v>637</v>
+      </c>
+      <c r="D910" s="7" t="s">
+        <v>638</v>
+      </c>
+      <c r="E910" s="7">
+        <v>3</v>
+      </c>
+      <c r="F910" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G910" s="7">
+        <v>512</v>
+      </c>
+      <c r="H910" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I910" s="7"/>
+      <c r="J910" s="7"/>
+    </row>
+    <row r="911" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B911" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="C911" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="D911" s="7" t="s">
+        <v>639</v>
+      </c>
+      <c r="E911" s="7">
+        <v>4</v>
+      </c>
+      <c r="F911" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G911" s="7">
+        <v>256</v>
+      </c>
+      <c r="H911" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I911" s="7"/>
+      <c r="J911" s="7"/>
+    </row>
+    <row r="912" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B912" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="C912" s="7" t="s">
+        <v>640</v>
+      </c>
+      <c r="D912" s="7" t="s">
+        <v>641</v>
+      </c>
+      <c r="E912" s="7">
+        <v>5</v>
+      </c>
+      <c r="F912" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G912" s="7">
+        <v>16</v>
+      </c>
+      <c r="H912" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I912" s="7"/>
+      <c r="J912" s="7"/>
+    </row>
+    <row r="913" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B913" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="C913" s="7" t="s">
+        <v>642</v>
+      </c>
+      <c r="D913" s="7" t="s">
+        <v>643</v>
+      </c>
+      <c r="E913" s="7">
+        <v>6</v>
+      </c>
+      <c r="F913" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G913" s="7">
+        <v>36</v>
+      </c>
+      <c r="H913" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I913" s="7"/>
+      <c r="J913" s="7"/>
+    </row>
+    <row r="914" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B914" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="C914" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D914" s="7" t="s">
+        <v>644</v>
+      </c>
+      <c r="E914" s="7">
+        <v>7</v>
+      </c>
+      <c r="F914" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G914" s="7"/>
+      <c r="H914" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I914" s="7"/>
+      <c r="J914" s="7"/>
+    </row>
+    <row r="915" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B915" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="C915" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D915" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E915" s="7">
+        <v>8</v>
+      </c>
+      <c r="F915" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G915" s="7">
+        <v>256</v>
+      </c>
+      <c r="H915" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I915" s="7"/>
+      <c r="J915" s="7"/>
+    </row>
+    <row r="916" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B916" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="C916" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D916" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E916" s="7">
+        <v>9</v>
+      </c>
+      <c r="F916" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G916" s="7"/>
+      <c r="H916" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I916" s="7"/>
+      <c r="J916" s="7"/>
+    </row>
+    <row r="917" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B917" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="C917" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D917" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E917" s="7">
+        <v>10</v>
+      </c>
+      <c r="F917" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G917" s="7">
+        <v>256</v>
+      </c>
+      <c r="H917" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I917" s="7"/>
+      <c r="J917" s="7"/>
+    </row>
+    <row r="918" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B918" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="C918" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D918" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E918" s="7">
+        <v>11</v>
+      </c>
+      <c r="F918" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G918" s="7"/>
+      <c r="H918" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I918" s="7"/>
+      <c r="J918" s="7"/>
+    </row>
+    <row r="919" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B919" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="C919" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D919" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E919" s="7">
+        <v>12</v>
+      </c>
+      <c r="F919" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G919" s="7"/>
+      <c r="H919" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I919" s="7"/>
+      <c r="J919" s="7"/>
+    </row>
+    <row r="920" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B920" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="C920" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D920" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E920" s="7">
+        <v>13</v>
+      </c>
+      <c r="F920" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G920" s="7"/>
+      <c r="H920" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I920" s="7"/>
+      <c r="J920" s="7"/>
+    </row>
+    <row r="921" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B921" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="C921" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="D921" s="5"/>
+      <c r="E921" s="5"/>
+      <c r="F921" s="5"/>
+      <c r="G921" s="5"/>
+      <c r="H921" s="5"/>
+      <c r="I921" s="5"/>
+      <c r="J921" s="5"/>
+    </row>
+    <row r="922" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B922" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="C922" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D922" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="E922" s="7">
+        <v>1</v>
+      </c>
+      <c r="F922" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G922" s="7">
+        <v>36</v>
+      </c>
+      <c r="H922" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I922" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="J922" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="923" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B923" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="C923" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="D923" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="E923" s="7">
+        <v>2</v>
+      </c>
+      <c r="F923" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G923" s="7">
+        <v>128</v>
+      </c>
+      <c r="H923" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I923" s="7"/>
+      <c r="J923" s="7"/>
+    </row>
+    <row r="924" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B924" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="C924" s="7" t="s">
+        <v>637</v>
+      </c>
+      <c r="D924" s="7" t="s">
+        <v>638</v>
+      </c>
+      <c r="E924" s="7">
+        <v>3</v>
+      </c>
+      <c r="F924" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G924" s="7">
+        <v>512</v>
+      </c>
+      <c r="H924" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I924" s="7"/>
+      <c r="J924" s="7"/>
+    </row>
+    <row r="925" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B925" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="C925" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="D925" s="7" t="s">
+        <v>639</v>
+      </c>
+      <c r="E925" s="7">
+        <v>4</v>
+      </c>
+      <c r="F925" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G925" s="7">
+        <v>256</v>
+      </c>
+      <c r="H925" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I925" s="7"/>
+      <c r="J925" s="7"/>
+    </row>
+    <row r="926" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B926" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="C926" s="7" t="s">
+        <v>640</v>
+      </c>
+      <c r="D926" s="7" t="s">
+        <v>641</v>
+      </c>
+      <c r="E926" s="7">
+        <v>5</v>
+      </c>
+      <c r="F926" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G926" s="7">
+        <v>16</v>
+      </c>
+      <c r="H926" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I926" s="7"/>
+      <c r="J926" s="7"/>
+    </row>
+    <row r="927" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B927" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="C927" s="7" t="s">
+        <v>642</v>
+      </c>
+      <c r="D927" s="7" t="s">
+        <v>643</v>
+      </c>
+      <c r="E927" s="7">
+        <v>6</v>
+      </c>
+      <c r="F927" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G927" s="7">
+        <v>36</v>
+      </c>
+      <c r="H927" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I927" s="7"/>
+      <c r="J927" s="7"/>
+    </row>
+    <row r="928" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B928" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="C928" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D928" s="7" t="s">
+        <v>644</v>
+      </c>
+      <c r="E928" s="7">
+        <v>7</v>
+      </c>
+      <c r="F928" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G928" s="7"/>
+      <c r="H928" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I928" s="7"/>
+      <c r="J928" s="7"/>
+    </row>
+    <row r="929" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B929" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="C929" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D929" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E929" s="7">
+        <v>8</v>
+      </c>
+      <c r="F929" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G929" s="7">
+        <v>256</v>
+      </c>
+      <c r="H929" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I929" s="7"/>
+      <c r="J929" s="7"/>
+    </row>
+    <row r="930" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B930" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="C930" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D930" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E930" s="7">
+        <v>9</v>
+      </c>
+      <c r="F930" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G930" s="7"/>
+      <c r="H930" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I930" s="7"/>
+      <c r="J930" s="7"/>
+    </row>
+    <row r="931" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B931" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="C931" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D931" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E931" s="7">
+        <v>10</v>
+      </c>
+      <c r="F931" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G931" s="7">
+        <v>256</v>
+      </c>
+      <c r="H931" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I931" s="7"/>
+      <c r="J931" s="7"/>
+    </row>
+    <row r="932" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B932" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="C932" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D932" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E932" s="7">
+        <v>11</v>
+      </c>
+      <c r="F932" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G932" s="7"/>
+      <c r="H932" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I932" s="7"/>
+      <c r="J932" s="7"/>
+    </row>
+    <row r="933" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B933" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="C933" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D933" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E933" s="7">
+        <v>12</v>
+      </c>
+      <c r="F933" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G933" s="7"/>
+      <c r="H933" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I933" s="7"/>
+      <c r="J933" s="7"/>
+    </row>
+    <row r="934" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B934" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="C934" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D934" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E934" s="7">
+        <v>13</v>
+      </c>
+      <c r="F934" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G934" s="7"/>
+      <c r="H934" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I934" s="7"/>
+      <c r="J934" s="7"/>
+    </row>
+    <row r="935" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B935" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="C935" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="D935" s="7" t="s">
+        <v>646</v>
+      </c>
+      <c r="E935" s="7">
+        <v>14</v>
+      </c>
+      <c r="F935" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G935" s="7"/>
+      <c r="H935" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I935" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="J935" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="936" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B936" s="5" t="s">
+        <v>611</v>
+      </c>
+      <c r="C936" s="5" t="s">
+        <v>612</v>
+      </c>
+      <c r="D936" s="5"/>
+      <c r="E936" s="5"/>
+      <c r="F936" s="5"/>
+      <c r="G936" s="5"/>
+      <c r="H936" s="5"/>
+      <c r="I936" s="5"/>
+      <c r="J936" s="5"/>
+    </row>
+    <row r="937" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B937" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="C937" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D937" s="7" t="s">
+        <v>648</v>
+      </c>
+      <c r="E937" s="7">
+        <v>1</v>
+      </c>
+      <c r="F937" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G937" s="7">
+        <v>36</v>
+      </c>
+      <c r="H937" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I937" s="7" t="s">
+        <v>647</v>
+      </c>
+      <c r="J937" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="938" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B938" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="C938" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D938" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="E938" s="7">
+        <v>2</v>
+      </c>
+      <c r="F938" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G938" s="7">
+        <v>128</v>
+      </c>
+      <c r="H938" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I938" s="7"/>
+      <c r="J938" s="7"/>
+    </row>
+    <row r="939" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B939" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="C939" s="7" t="s">
+        <v>637</v>
+      </c>
+      <c r="D939" s="7" t="s">
+        <v>650</v>
+      </c>
+      <c r="E939" s="7">
+        <v>3</v>
+      </c>
+      <c r="F939" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G939" s="7">
+        <v>512</v>
+      </c>
+      <c r="H939" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I939" s="7"/>
+      <c r="J939" s="7"/>
+    </row>
+    <row r="940" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B940" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="C940" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="D940" s="7" t="s">
+        <v>651</v>
+      </c>
+      <c r="E940" s="7">
+        <v>4</v>
+      </c>
+      <c r="F940" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G940" s="7">
+        <v>256</v>
+      </c>
+      <c r="H940" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I940" s="7"/>
+      <c r="J940" s="7"/>
+    </row>
+    <row r="941" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B941" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="C941" s="7" t="s">
+        <v>640</v>
+      </c>
+      <c r="D941" s="7" t="s">
+        <v>652</v>
+      </c>
+      <c r="E941" s="7">
+        <v>5</v>
+      </c>
+      <c r="F941" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G941" s="7">
+        <v>16</v>
+      </c>
+      <c r="H941" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I941" s="7"/>
+      <c r="J941" s="7"/>
+    </row>
+    <row r="942" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B942" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="C942" s="7" t="s">
+        <v>642</v>
+      </c>
+      <c r="D942" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="E942" s="7">
+        <v>6</v>
+      </c>
+      <c r="F942" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G942" s="7">
+        <v>36</v>
+      </c>
+      <c r="H942" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I942" s="7"/>
+      <c r="J942" s="7"/>
+    </row>
+    <row r="943" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B943" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="C943" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D943" s="7" t="s">
+        <v>644</v>
+      </c>
+      <c r="E943" s="7">
+        <v>7</v>
+      </c>
+      <c r="F943" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G943" s="7"/>
+      <c r="H943" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I943" s="7"/>
+      <c r="J943" s="7"/>
+    </row>
+    <row r="944" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B944" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="C944" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D944" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E944" s="7">
+        <v>8</v>
+      </c>
+      <c r="F944" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G944" s="7">
+        <v>256</v>
+      </c>
+      <c r="H944" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I944" s="7"/>
+      <c r="J944" s="7"/>
+    </row>
+    <row r="945" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B945" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="C945" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D945" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E945" s="7">
+        <v>9</v>
+      </c>
+      <c r="F945" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G945" s="7"/>
+      <c r="H945" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I945" s="7"/>
+      <c r="J945" s="7"/>
+    </row>
+    <row r="946" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B946" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="C946" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D946" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E946" s="7">
+        <v>10</v>
+      </c>
+      <c r="F946" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G946" s="7">
+        <v>256</v>
+      </c>
+      <c r="H946" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I946" s="7"/>
+      <c r="J946" s="7"/>
+    </row>
+    <row r="947" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B947" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="C947" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D947" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E947" s="7">
+        <v>11</v>
+      </c>
+      <c r="F947" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G947" s="7"/>
+      <c r="H947" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I947" s="7"/>
+      <c r="J947" s="7"/>
+    </row>
+    <row r="948" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B948" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="C948" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D948" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E948" s="7">
+        <v>12</v>
+      </c>
+      <c r="F948" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G948" s="7"/>
+      <c r="H948" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I948" s="7"/>
+      <c r="J948" s="7"/>
+    </row>
+    <row r="949" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B949" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="C949" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D949" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E949" s="7">
+        <v>13</v>
+      </c>
+      <c r="F949" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G949" s="7"/>
+      <c r="H949" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I949" s="7"/>
+      <c r="J949" s="7"/>
+    </row>
+    <row r="950" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B950" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="C950" s="5" t="s">
+        <v>614</v>
+      </c>
+      <c r="D950" s="5"/>
+      <c r="E950" s="5"/>
+      <c r="F950" s="5"/>
+      <c r="G950" s="5"/>
+      <c r="H950" s="5"/>
+      <c r="I950" s="5"/>
+      <c r="J950" s="5"/>
+    </row>
+    <row r="951" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B951" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C951" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D951" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="E951" s="7">
+        <v>1</v>
+      </c>
+      <c r="F951" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G951" s="7">
+        <v>36</v>
+      </c>
+      <c r="H951" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I951" s="7" t="s">
+        <v>654</v>
+      </c>
+      <c r="J951" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="952" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B952" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C952" s="7" t="s">
+        <v>656</v>
+      </c>
+      <c r="D952" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="E952" s="7">
+        <v>2</v>
+      </c>
+      <c r="F952" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="G952" s="7"/>
+      <c r="H952" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I952" s="7"/>
+      <c r="J952" s="7"/>
+    </row>
+    <row r="953" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B953" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C953" s="7" t="s">
+        <v>658</v>
+      </c>
+      <c r="D953" s="7" t="s">
+        <v>661</v>
+      </c>
+      <c r="E953" s="7">
+        <v>3</v>
+      </c>
+      <c r="F953" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G953" s="7">
+        <v>64</v>
+      </c>
+      <c r="H953" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I953" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="J953" s="7" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="954" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B954" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C954" s="7" t="s">
+        <v>662</v>
+      </c>
+      <c r="D954" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="E954" s="7">
+        <v>4</v>
+      </c>
+      <c r="F954" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G954" s="7">
+        <v>36</v>
+      </c>
+      <c r="H954" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I954" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="J954" s="7" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="955" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B955" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C955" s="7" t="s">
+        <v>666</v>
+      </c>
+      <c r="D955" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="E955" s="7">
+        <v>5</v>
+      </c>
+      <c r="F955" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G955" s="7">
+        <v>36</v>
+      </c>
+      <c r="H955" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I955" s="7" t="s">
+        <v>667</v>
+      </c>
+      <c r="J955" s="7" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="956" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B956" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C956" s="7" t="s">
+        <v>670</v>
+      </c>
+      <c r="D956" s="7" t="s">
+        <v>672</v>
+      </c>
+      <c r="E956" s="7">
+        <v>6</v>
+      </c>
+      <c r="F956" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G956" s="7">
+        <v>36</v>
+      </c>
+      <c r="H956" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I956" s="7" t="s">
+        <v>671</v>
+      </c>
+      <c r="J956" s="7" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="957" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B957" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C957" s="7" t="s">
+        <v>673</v>
+      </c>
+      <c r="D957" s="7" t="s">
+        <v>674</v>
+      </c>
+      <c r="E957" s="7">
+        <v>7</v>
+      </c>
+      <c r="F957" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G957" s="7">
+        <v>36</v>
+      </c>
+      <c r="H957" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I957" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="J957" s="7" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="958" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B958" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C958" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="D958" s="7" t="s">
+        <v>675</v>
+      </c>
+      <c r="E958" s="7">
+        <v>8</v>
+      </c>
+      <c r="F958" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G958" s="7">
+        <v>36</v>
+      </c>
+      <c r="H958" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I958" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="J958" s="7" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="959" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B959" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C959" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="D959" s="7" t="s">
+        <v>677</v>
+      </c>
+      <c r="E959" s="7">
+        <v>9</v>
+      </c>
+      <c r="F959" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G959" s="7"/>
+      <c r="H959" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I959" s="7"/>
+      <c r="J959" s="7"/>
+    </row>
+    <row r="960" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B960" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C960" s="7" t="s">
+        <v>678</v>
+      </c>
+      <c r="D960" s="7" t="s">
+        <v>679</v>
+      </c>
+      <c r="E960" s="7">
+        <v>10</v>
+      </c>
+      <c r="F960" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G960" s="7"/>
+      <c r="H960" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I960" s="7"/>
+      <c r="J960" s="7"/>
+    </row>
+    <row r="961" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B961" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C961" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D961" s="7" t="s">
+        <v>644</v>
+      </c>
+      <c r="E961" s="7">
+        <v>11</v>
+      </c>
+      <c r="F961" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G961" s="7"/>
+      <c r="H961" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I961" s="7"/>
+      <c r="J961" s="7"/>
+    </row>
+    <row r="962" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B962" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C962" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D962" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E962" s="7">
+        <v>12</v>
+      </c>
+      <c r="F962" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G962" s="7">
+        <v>256</v>
+      </c>
+      <c r="H962" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I962" s="7"/>
+      <c r="J962" s="7"/>
+    </row>
+    <row r="963" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B963" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C963" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D963" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E963" s="7">
+        <v>13</v>
+      </c>
+      <c r="F963" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G963" s="7"/>
+      <c r="H963" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I963" s="7"/>
+      <c r="J963" s="7"/>
+    </row>
+    <row r="964" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B964" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C964" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D964" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E964" s="7">
+        <v>14</v>
+      </c>
+      <c r="F964" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G964" s="7">
+        <v>256</v>
+      </c>
+      <c r="H964" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I964" s="7"/>
+      <c r="J964" s="7"/>
+    </row>
+    <row r="965" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B965" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C965" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D965" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E965" s="7">
+        <v>15</v>
+      </c>
+      <c r="F965" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G965" s="7"/>
+      <c r="H965" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I965" s="7"/>
+      <c r="J965" s="7"/>
+    </row>
+    <row r="966" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B966" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C966" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D966" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E966" s="7">
+        <v>16</v>
+      </c>
+      <c r="F966" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G966" s="7"/>
+      <c r="H966" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I966" s="7"/>
+      <c r="J966" s="7"/>
+    </row>
+    <row r="967" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B967" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C967" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D967" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E967" s="7">
+        <v>17</v>
+      </c>
+      <c r="F967" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G967" s="7"/>
+      <c r="H967" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I967" s="7"/>
+      <c r="J967" s="7"/>
+    </row>
+    <row r="968" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B968" s="5" t="s">
+        <v>615</v>
+      </c>
+      <c r="C968" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="D968" s="5"/>
+      <c r="E968" s="5"/>
+      <c r="F968" s="5"/>
+      <c r="G968" s="5"/>
+      <c r="H968" s="5"/>
+      <c r="I968" s="5"/>
+      <c r="J968" s="5"/>
+    </row>
+    <row r="969" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B969" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="C969" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D969" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="E969" s="7">
+        <v>1</v>
+      </c>
+      <c r="F969" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G969" s="7">
+        <v>36</v>
+      </c>
+      <c r="H969" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I969" s="7" t="s">
+        <v>680</v>
+      </c>
+      <c r="J969" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="970" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B970" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="C970" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D970" s="7" t="s">
+        <v>682</v>
+      </c>
+      <c r="E970" s="7">
+        <v>2</v>
+      </c>
+      <c r="F970" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G970" s="7">
+        <v>64</v>
+      </c>
+      <c r="H970" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I970" s="7"/>
+      <c r="J970" s="7"/>
+    </row>
+    <row r="971" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B971" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="C971" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D971" s="7" t="s">
+        <v>683</v>
+      </c>
+      <c r="E971" s="7">
+        <v>3</v>
+      </c>
+      <c r="F971" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G971" s="7">
+        <v>512</v>
+      </c>
+      <c r="H971" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I971" s="7"/>
+      <c r="J971" s="7"/>
+    </row>
+    <row r="972" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B972" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="C972" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D972" s="7" t="s">
+        <v>644</v>
+      </c>
+      <c r="E972" s="7">
+        <v>4</v>
+      </c>
+      <c r="F972" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G972" s="7"/>
+      <c r="H972" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I972" s="7"/>
+      <c r="J972" s="7"/>
+    </row>
+    <row r="973" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B973" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="C973" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D973" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E973" s="7">
+        <v>5</v>
+      </c>
+      <c r="F973" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G973" s="7">
+        <v>256</v>
+      </c>
+      <c r="H973" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I973" s="7"/>
+      <c r="J973" s="7"/>
+    </row>
+    <row r="974" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B974" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="C974" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D974" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E974" s="7">
+        <v>6</v>
+      </c>
+      <c r="F974" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G974" s="7"/>
+      <c r="H974" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I974" s="7"/>
+      <c r="J974" s="7"/>
+    </row>
+    <row r="975" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B975" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="C975" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D975" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E975" s="7">
+        <v>7</v>
+      </c>
+      <c r="F975" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G975" s="7">
+        <v>256</v>
+      </c>
+      <c r="H975" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I975" s="7"/>
+      <c r="J975" s="7"/>
+    </row>
+    <row r="976" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B976" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="C976" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D976" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E976" s="7">
+        <v>8</v>
+      </c>
+      <c r="F976" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G976" s="7"/>
+      <c r="H976" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I976" s="7"/>
+      <c r="J976" s="7"/>
+    </row>
+    <row r="977" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B977" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="C977" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D977" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E977" s="7">
+        <v>9</v>
+      </c>
+      <c r="F977" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G977" s="7"/>
+      <c r="H977" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I977" s="7"/>
+      <c r="J977" s="7"/>
+    </row>
+    <row r="978" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B978" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="C978" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D978" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E978" s="7">
+        <v>10</v>
+      </c>
+      <c r="F978" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G978" s="7"/>
+      <c r="H978" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I978" s="7"/>
+      <c r="J978" s="7"/>
+    </row>
+    <row r="979" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B979" s="5" t="s">
+        <v>617</v>
+      </c>
+      <c r="C979" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="D979" s="5"/>
+      <c r="E979" s="5"/>
+      <c r="F979" s="5"/>
+      <c r="G979" s="5"/>
+      <c r="H979" s="5"/>
+      <c r="I979" s="5"/>
+      <c r="J979" s="5"/>
+    </row>
+    <row r="980" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B980" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C980" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="D980" s="7" t="s">
+        <v>685</v>
+      </c>
+      <c r="E980" s="7">
+        <v>1</v>
+      </c>
+      <c r="F980" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G980" s="7">
+        <v>10</v>
+      </c>
+      <c r="H980" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I980" s="7" t="s">
+        <v>684</v>
+      </c>
+      <c r="J980" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="981" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B981" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C981" s="7" t="s">
+        <v>686</v>
+      </c>
+      <c r="D981" s="7" t="s">
+        <v>688</v>
+      </c>
+      <c r="E981" s="7">
+        <v>2</v>
+      </c>
+      <c r="F981" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="G981" s="7"/>
+      <c r="H981" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I981" s="7" t="s">
+        <v>687</v>
+      </c>
+      <c r="J981" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="982" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B982" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C982" s="7" t="s">
+        <v>689</v>
+      </c>
+      <c r="D982" s="7" t="s">
+        <v>690</v>
+      </c>
+      <c r="E982" s="7">
+        <v>3</v>
+      </c>
+      <c r="F982" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G982" s="7">
+        <v>128</v>
+      </c>
+      <c r="H982" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I982" s="7"/>
+      <c r="J982" s="7"/>
+    </row>
+    <row r="983" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B983" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C983" s="7" t="s">
+        <v>691</v>
+      </c>
+      <c r="D983" s="7" t="s">
+        <v>692</v>
+      </c>
+      <c r="E983" s="7">
+        <v>4</v>
+      </c>
+      <c r="F983" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G983" s="7">
+        <v>256</v>
+      </c>
+      <c r="H983" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I983" s="7"/>
+      <c r="J983" s="7"/>
+    </row>
+    <row r="984" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B984" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C984" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D984" s="7" t="s">
+        <v>632</v>
+      </c>
+      <c r="E984" s="7">
+        <v>5</v>
+      </c>
+      <c r="F984" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G984" s="7">
+        <v>3</v>
+      </c>
+      <c r="H984" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I984" s="7" t="s">
+        <v>693</v>
+      </c>
+      <c r="J984" s="7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="985" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B985" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C985" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D985" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E985" s="7">
+        <v>6</v>
+      </c>
+      <c r="F985" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G985" s="7"/>
+      <c r="H985" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I985" s="7"/>
+      <c r="J985" s="7"/>
+    </row>
+    <row r="986" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B986" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C986" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D986" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E986" s="7">
+        <v>7</v>
+      </c>
+      <c r="F986" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G986" s="7">
+        <v>256</v>
+      </c>
+      <c r="H986" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I986" s="7"/>
+      <c r="J986" s="7"/>
+    </row>
+    <row r="987" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B987" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C987" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D987" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E987" s="7">
+        <v>8</v>
+      </c>
+      <c r="F987" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G987" s="7"/>
+      <c r="H987" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I987" s="7"/>
+      <c r="J987" s="7"/>
+    </row>
+    <row r="988" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B988" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C988" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D988" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E988" s="7">
+        <v>9</v>
+      </c>
+      <c r="F988" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G988" s="7">
+        <v>256</v>
+      </c>
+      <c r="H988" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I988" s="7"/>
+      <c r="J988" s="7"/>
+    </row>
+    <row r="989" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B989" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C989" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D989" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E989" s="7">
+        <v>10</v>
+      </c>
+      <c r="F989" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G989" s="7"/>
+      <c r="H989" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I989" s="7"/>
+      <c r="J989" s="7"/>
+    </row>
+    <row r="990" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B990" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C990" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D990" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E990" s="7">
+        <v>11</v>
+      </c>
+      <c r="F990" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G990" s="7"/>
+      <c r="H990" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I990" s="7"/>
+      <c r="J990" s="7"/>
+    </row>
+    <row r="991" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B991" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C991" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D991" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E991" s="7">
+        <v>12</v>
+      </c>
+      <c r="F991" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G991" s="7"/>
+      <c r="H991" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I991" s="7"/>
+      <c r="J991" s="7"/>
+    </row>
+    <row r="992" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B992" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="C992" s="5" t="s">
+        <v>620</v>
+      </c>
+      <c r="D992" s="5"/>
+      <c r="E992" s="5"/>
+      <c r="F992" s="5"/>
+      <c r="G992" s="5"/>
+      <c r="H992" s="5"/>
+      <c r="I992" s="5"/>
+      <c r="J992" s="5"/>
+    </row>
+    <row r="993" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B993" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C993" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D993" s="7" t="s">
+        <v>695</v>
+      </c>
+      <c r="E993" s="7">
+        <v>1</v>
+      </c>
+      <c r="F993" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G993" s="7">
+        <v>36</v>
+      </c>
+      <c r="H993" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I993" s="7" t="s">
+        <v>694</v>
+      </c>
+      <c r="J993" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="994" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B994" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C994" s="7" t="s">
+        <v>666</v>
+      </c>
+      <c r="D994" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="E994" s="7">
+        <v>2</v>
+      </c>
+      <c r="F994" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G994" s="7">
+        <v>36</v>
+      </c>
+      <c r="H994" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I994" s="7" t="s">
+        <v>696</v>
+      </c>
+      <c r="J994" s="7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="995" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B995" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C995" s="7" t="s">
+        <v>670</v>
+      </c>
+      <c r="D995" s="7" t="s">
+        <v>698</v>
+      </c>
+      <c r="E995" s="7">
+        <v>3</v>
+      </c>
+      <c r="F995" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G995" s="7">
+        <v>36</v>
+      </c>
+      <c r="H995" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I995" s="7" t="s">
+        <v>697</v>
+      </c>
+      <c r="J995" s="7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="996" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B996" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C996" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="D996" s="7" t="s">
+        <v>699</v>
+      </c>
+      <c r="E996" s="7">
+        <v>4</v>
+      </c>
+      <c r="F996" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G996" s="7">
+        <v>64</v>
+      </c>
+      <c r="H996" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I996" s="7"/>
+      <c r="J996" s="7"/>
+    </row>
+    <row r="997" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B997" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C997" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="D997" s="7" t="s">
+        <v>700</v>
+      </c>
+      <c r="E997" s="7">
+        <v>5</v>
+      </c>
+      <c r="F997" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G997" s="7">
+        <v>256</v>
+      </c>
+      <c r="H997" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I997" s="7"/>
+      <c r="J997" s="7"/>
+    </row>
+    <row r="998" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B998" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C998" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="D998" s="7" t="s">
+        <v>702</v>
+      </c>
+      <c r="E998" s="7">
+        <v>6</v>
+      </c>
+      <c r="F998" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G998" s="7">
+        <v>256</v>
+      </c>
+      <c r="H998" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I998" s="7"/>
+      <c r="J998" s="7"/>
+    </row>
+    <row r="999" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B999" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C999" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="D999" s="7" t="s">
+        <v>704</v>
+      </c>
+      <c r="E999" s="7">
+        <v>7</v>
+      </c>
+      <c r="F999" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G999" s="7">
+        <v>1024</v>
+      </c>
+      <c r="H999" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I999" s="7"/>
+      <c r="J999" s="7"/>
+    </row>
+    <row r="1000" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1000" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1000" s="7" t="s">
+        <v>705</v>
+      </c>
+      <c r="D1000" s="7" t="s">
+        <v>707</v>
+      </c>
+      <c r="E1000" s="7">
+        <v>8</v>
+      </c>
+      <c r="F1000" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1000" s="7">
+        <v>64</v>
+      </c>
+      <c r="H1000" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1000" s="7" t="s">
+        <v>706</v>
+      </c>
+      <c r="J1000" s="7" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="1001" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1001" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1001" s="7" t="s">
+        <v>708</v>
+      </c>
+      <c r="D1001" s="7" t="s">
+        <v>710</v>
+      </c>
+      <c r="E1001" s="7">
+        <v>9</v>
+      </c>
+      <c r="F1001" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1001" s="7">
+        <v>36</v>
+      </c>
+      <c r="H1001" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1001" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="J1001" s="7" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="1002" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1002" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1002" s="7" t="s">
+        <v>711</v>
+      </c>
+      <c r="D1002" s="7" t="s">
+        <v>712</v>
+      </c>
+      <c r="E1002" s="7">
+        <v>10</v>
+      </c>
+      <c r="F1002" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1002" s="7">
+        <v>128</v>
+      </c>
+      <c r="H1002" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1002" s="7"/>
+      <c r="J1002" s="7"/>
+    </row>
+    <row r="1003" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1003" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1003" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="D1003" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="E1003" s="7">
+        <v>11</v>
+      </c>
+      <c r="F1003" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1003" s="7">
+        <v>64</v>
+      </c>
+      <c r="H1003" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1003" s="7"/>
+      <c r="J1003" s="7"/>
+    </row>
+    <row r="1004" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1004" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1004" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="D1004" s="7" t="s">
+        <v>716</v>
+      </c>
+      <c r="E1004" s="7">
+        <v>12</v>
+      </c>
+      <c r="F1004" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1004" s="7">
+        <v>128</v>
+      </c>
+      <c r="H1004" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1004" s="7"/>
+      <c r="J1004" s="7"/>
+    </row>
+    <row r="1005" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1005" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1005" s="7" t="s">
+        <v>673</v>
+      </c>
+      <c r="D1005" s="7" t="s">
+        <v>674</v>
+      </c>
+      <c r="E1005" s="7">
+        <v>13</v>
+      </c>
+      <c r="F1005" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1005" s="7">
+        <v>36</v>
+      </c>
+      <c r="H1005" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1005" s="7"/>
+      <c r="J1005" s="7"/>
+    </row>
+    <row r="1006" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1006" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1006" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="D1006" s="7"/>
+      <c r="E1006" s="7">
+        <v>14</v>
+      </c>
+      <c r="F1006" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1006" s="7">
+        <v>36</v>
+      </c>
+      <c r="H1006" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1006" s="7"/>
+      <c r="J1006" s="7"/>
+    </row>
+    <row r="1007" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1007" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1007" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="D1007" s="7" t="s">
+        <v>718</v>
+      </c>
+      <c r="E1007" s="7">
+        <v>15</v>
+      </c>
+      <c r="F1007" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1007" s="7"/>
+      <c r="H1007" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1007" s="7"/>
+      <c r="J1007" s="7"/>
+    </row>
+    <row r="1008" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1008" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1008" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="D1008" s="7" t="s">
+        <v>720</v>
+      </c>
+      <c r="E1008" s="7">
+        <v>16</v>
+      </c>
+      <c r="F1008" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1008" s="7">
+        <v>3</v>
+      </c>
+      <c r="H1008" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1008" s="7"/>
+      <c r="J1008" s="7"/>
+    </row>
+    <row r="1009" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1009" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1009" s="7" t="s">
+        <v>721</v>
+      </c>
+      <c r="D1009" s="7" t="s">
+        <v>722</v>
+      </c>
+      <c r="E1009" s="7">
+        <v>17</v>
+      </c>
+      <c r="F1009" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1009" s="7">
+        <v>36</v>
+      </c>
+      <c r="H1009" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1009" s="7"/>
+      <c r="J1009" s="7"/>
+    </row>
+    <row r="1010" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1010" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1010" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1010" s="7" t="s">
+        <v>644</v>
+      </c>
+      <c r="E1010" s="7">
+        <v>21</v>
+      </c>
+      <c r="F1010" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1010" s="7"/>
+      <c r="H1010" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1010" s="7"/>
+      <c r="J1010" s="7"/>
+    </row>
+    <row r="1011" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1011" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1011" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1011" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1011" s="7">
+        <v>22</v>
+      </c>
+      <c r="F1011" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1011" s="7">
+        <v>256</v>
+      </c>
+      <c r="H1011" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1011" s="7"/>
+      <c r="J1011" s="7"/>
+    </row>
+    <row r="1012" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1012" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1012" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1012" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1012" s="7">
+        <v>23</v>
+      </c>
+      <c r="F1012" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1012" s="7"/>
+      <c r="H1012" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1012" s="7"/>
+      <c r="J1012" s="7"/>
+    </row>
+    <row r="1013" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1013" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1013" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1013" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1013" s="7">
+        <v>24</v>
+      </c>
+      <c r="F1013" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1013" s="7">
+        <v>256</v>
+      </c>
+      <c r="H1013" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1013" s="7"/>
+      <c r="J1013" s="7"/>
+    </row>
+    <row r="1014" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1014" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1014" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1014" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1014" s="7">
+        <v>25</v>
+      </c>
+      <c r="F1014" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1014" s="7"/>
+      <c r="H1014" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1014" s="7"/>
+      <c r="J1014" s="7"/>
+    </row>
+    <row r="1015" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1015" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1015" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1015" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1015" s="7">
+        <v>26</v>
+      </c>
+      <c r="F1015" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1015" s="7"/>
+      <c r="H1015" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1015" s="7"/>
+      <c r="J1015" s="7"/>
+    </row>
+    <row r="1016" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1016" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1016" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1016" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1016" s="7">
+        <v>27</v>
+      </c>
+      <c r="F1016" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1016" s="7"/>
+      <c r="H1016" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1016" s="7"/>
+      <c r="J1016" s="7"/>
+    </row>
+    <row r="1017" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1017" s="5" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1017" s="5" t="s">
+        <v>622</v>
+      </c>
+      <c r="D1017" s="5"/>
+      <c r="E1017" s="5"/>
+      <c r="F1017" s="5"/>
+      <c r="G1017" s="5"/>
+      <c r="H1017" s="5"/>
+      <c r="I1017" s="5"/>
+      <c r="J1017" s="5"/>
+    </row>
+    <row r="1018" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1018" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1018" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1018" s="7" t="s">
+        <v>695</v>
+      </c>
+      <c r="E1018" s="7">
+        <v>1</v>
+      </c>
+      <c r="F1018" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1018" s="7">
+        <v>36</v>
+      </c>
+      <c r="H1018" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1018" s="7" t="s">
+        <v>723</v>
+      </c>
+      <c r="J1018" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="1019" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1019" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1019" s="7" t="s">
+        <v>666</v>
+      </c>
+      <c r="D1019" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="E1019" s="7">
+        <v>2</v>
+      </c>
+      <c r="F1019" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1019" s="7">
+        <v>36</v>
+      </c>
+      <c r="H1019" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1019" s="7"/>
+      <c r="J1019" s="7"/>
+    </row>
+    <row r="1020" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1020" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1020" s="7" t="s">
+        <v>670</v>
+      </c>
+      <c r="D1020" s="7" t="s">
+        <v>698</v>
+      </c>
+      <c r="E1020" s="7">
+        <v>3</v>
+      </c>
+      <c r="F1020" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1020" s="7">
+        <v>36</v>
+      </c>
+      <c r="H1020" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1020" s="7"/>
+      <c r="J1020" s="7"/>
+    </row>
+    <row r="1021" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1021" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1021" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="D1021" s="7" t="s">
+        <v>699</v>
+      </c>
+      <c r="E1021" s="7">
+        <v>4</v>
+      </c>
+      <c r="F1021" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1021" s="7">
+        <v>64</v>
+      </c>
+      <c r="H1021" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1021" s="7"/>
+      <c r="J1021" s="7"/>
+    </row>
+    <row r="1022" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1022" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1022" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="D1022" s="7" t="s">
+        <v>700</v>
+      </c>
+      <c r="E1022" s="7">
+        <v>5</v>
+      </c>
+      <c r="F1022" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1022" s="7">
+        <v>256</v>
+      </c>
+      <c r="H1022" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1022" s="7"/>
+      <c r="J1022" s="7"/>
+    </row>
+    <row r="1023" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1023" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1023" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="D1023" s="7" t="s">
+        <v>702</v>
+      </c>
+      <c r="E1023" s="7">
+        <v>6</v>
+      </c>
+      <c r="F1023" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1023" s="7">
+        <v>1024</v>
+      </c>
+      <c r="H1023" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1023" s="7"/>
+      <c r="J1023" s="7"/>
+    </row>
+    <row r="1024" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1024" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1024" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="D1024" s="7" t="s">
+        <v>704</v>
+      </c>
+      <c r="E1024" s="7">
+        <v>7</v>
+      </c>
+      <c r="F1024" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1024" s="7">
+        <v>1024</v>
+      </c>
+      <c r="H1024" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1024" s="7"/>
+      <c r="J1024" s="7"/>
+    </row>
+    <row r="1025" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1025" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1025" s="7" t="s">
+        <v>705</v>
+      </c>
+      <c r="D1025" s="7" t="s">
+        <v>707</v>
+      </c>
+      <c r="E1025" s="7">
+        <v>8</v>
+      </c>
+      <c r="F1025" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1025" s="7">
+        <v>64</v>
+      </c>
+      <c r="H1025" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1025" s="7"/>
+      <c r="J1025" s="7"/>
+    </row>
+    <row r="1026" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1026" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1026" s="7" t="s">
+        <v>708</v>
+      </c>
+      <c r="D1026" s="7" t="s">
+        <v>710</v>
+      </c>
+      <c r="E1026" s="7">
+        <v>9</v>
+      </c>
+      <c r="F1026" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1026" s="7">
+        <v>36</v>
+      </c>
+      <c r="H1026" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1026" s="7"/>
+      <c r="J1026" s="7"/>
+    </row>
+    <row r="1027" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1027" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1027" s="7" t="s">
+        <v>711</v>
+      </c>
+      <c r="D1027" s="7" t="s">
+        <v>712</v>
+      </c>
+      <c r="E1027" s="7">
+        <v>10</v>
+      </c>
+      <c r="F1027" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1027" s="7">
+        <v>128</v>
+      </c>
+      <c r="H1027" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1027" s="7"/>
+      <c r="J1027" s="7"/>
+    </row>
+    <row r="1028" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1028" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1028" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="D1028" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="E1028" s="7">
+        <v>11</v>
+      </c>
+      <c r="F1028" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1028" s="7">
+        <v>64</v>
+      </c>
+      <c r="H1028" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1028" s="7"/>
+      <c r="J1028" s="7"/>
+    </row>
+    <row r="1029" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1029" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1029" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="D1029" s="7" t="s">
+        <v>716</v>
+      </c>
+      <c r="E1029" s="7">
+        <v>12</v>
+      </c>
+      <c r="F1029" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1029" s="7">
+        <v>128</v>
+      </c>
+      <c r="H1029" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1029" s="7"/>
+      <c r="J1029" s="7"/>
+    </row>
+    <row r="1030" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1030" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1030" s="7" t="s">
+        <v>673</v>
+      </c>
+      <c r="D1030" s="7" t="s">
+        <v>674</v>
+      </c>
+      <c r="E1030" s="7">
+        <v>13</v>
+      </c>
+      <c r="F1030" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1030" s="7">
+        <v>36</v>
+      </c>
+      <c r="H1030" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1030" s="7"/>
+      <c r="J1030" s="7"/>
+    </row>
+    <row r="1031" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1031" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1031" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="D1031" s="7"/>
+      <c r="E1031" s="7">
+        <v>14</v>
+      </c>
+      <c r="F1031" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1031" s="7">
+        <v>36</v>
+      </c>
+      <c r="H1031" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1031" s="7"/>
+      <c r="J1031" s="7"/>
+    </row>
+    <row r="1032" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1032" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1032" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="D1032" s="7" t="s">
+        <v>718</v>
+      </c>
+      <c r="E1032" s="7">
+        <v>15</v>
+      </c>
+      <c r="F1032" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1032" s="7"/>
+      <c r="H1032" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1032" s="7"/>
+      <c r="J1032" s="7"/>
+    </row>
+    <row r="1033" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1033" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1033" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="D1033" s="7" t="s">
+        <v>720</v>
+      </c>
+      <c r="E1033" s="7">
+        <v>16</v>
+      </c>
+      <c r="F1033" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1033" s="7">
+        <v>3</v>
+      </c>
+      <c r="H1033" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1033" s="7"/>
+      <c r="J1033" s="7"/>
+    </row>
+    <row r="1034" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1034" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1034" s="7" t="s">
+        <v>721</v>
+      </c>
+      <c r="D1034" s="7" t="s">
+        <v>722</v>
+      </c>
+      <c r="E1034" s="7">
+        <v>17</v>
+      </c>
+      <c r="F1034" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1034" s="7">
+        <v>36</v>
+      </c>
+      <c r="H1034" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1034" s="7"/>
+      <c r="J1034" s="7"/>
+    </row>
+    <row r="1035" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1035" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1035" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1035" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1035" s="7">
+        <v>21</v>
+      </c>
+      <c r="F1035" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1035" s="7"/>
+      <c r="H1035" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1035" s="7"/>
+      <c r="J1035" s="7"/>
+    </row>
+    <row r="1036" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1036" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1036" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1036" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1036" s="7">
+        <v>22</v>
+      </c>
+      <c r="F1036" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1036" s="7">
+        <v>256</v>
+      </c>
+      <c r="H1036" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1036" s="7"/>
+      <c r="J1036" s="7"/>
+    </row>
+    <row r="1037" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1037" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1037" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1037" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1037" s="7">
+        <v>23</v>
+      </c>
+      <c r="F1037" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1037" s="7"/>
+      <c r="H1037" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1037" s="7"/>
+      <c r="J1037" s="7"/>
+    </row>
+    <row r="1038" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1038" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1038" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1038" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1038" s="7">
+        <v>24</v>
+      </c>
+      <c r="F1038" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1038" s="7">
+        <v>256</v>
+      </c>
+      <c r="H1038" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1038" s="7"/>
+      <c r="J1038" s="7"/>
+    </row>
+    <row r="1039" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1039" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1039" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1039" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1039" s="7">
+        <v>25</v>
+      </c>
+      <c r="F1039" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1039" s="7"/>
+      <c r="H1039" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1039" s="7"/>
+      <c r="J1039" s="7"/>
+    </row>
+    <row r="1040" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1040" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1040" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1040" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1040" s="7">
+        <v>26</v>
+      </c>
+      <c r="F1040" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1040" s="7"/>
+      <c r="H1040" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1040" s="7"/>
+      <c r="J1040" s="7"/>
+    </row>
+    <row r="1041" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1041" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1041" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1041" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1041" s="7">
+        <v>27</v>
+      </c>
+      <c r="F1041" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1041" s="7"/>
+      <c r="H1041" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1041" s="7"/>
+      <c r="J1041" s="7"/>
+    </row>
+    <row r="1042" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1042" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1042" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1042" s="7" t="s">
+        <v>646</v>
+      </c>
+      <c r="E1042" s="7">
+        <v>28</v>
+      </c>
+      <c r="F1042" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1042" s="7"/>
+      <c r="H1042" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1042" s="7" t="s">
+        <v>723</v>
+      </c>
+      <c r="J1042" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="1043" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1043" s="5" t="s">
+        <v>623</v>
+      </c>
+      <c r="C1043" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="D1043" s="5"/>
+      <c r="E1043" s="5"/>
+      <c r="F1043" s="5"/>
+      <c r="G1043" s="5"/>
+      <c r="H1043" s="5"/>
+      <c r="I1043" s="5"/>
+      <c r="J1043" s="5"/>
+    </row>
+    <row r="1044" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1044" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="C1044" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="D1044" s="7" t="s">
+        <v>685</v>
+      </c>
+      <c r="E1044" s="7">
+        <v>1</v>
+      </c>
+      <c r="F1044" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1044" s="7">
+        <v>10</v>
+      </c>
+      <c r="H1044" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1044" s="7" t="s">
+        <v>724</v>
+      </c>
+      <c r="J1044" s="7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="1045" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1045" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="C1045" s="7" t="s">
+        <v>725</v>
+      </c>
+      <c r="D1045" s="7" t="s">
+        <v>727</v>
+      </c>
+      <c r="E1045" s="7">
+        <v>2</v>
+      </c>
+      <c r="F1045" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1045" s="7">
+        <v>3</v>
+      </c>
+      <c r="H1045" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1045" s="7" t="s">
+        <v>726</v>
+      </c>
+      <c r="J1045" s="7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="1046" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1046" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="C1046" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1046" s="7" t="s">
+        <v>632</v>
+      </c>
+      <c r="E1046" s="7">
+        <v>3</v>
+      </c>
+      <c r="F1046" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1046" s="7">
+        <v>3</v>
+      </c>
+      <c r="H1046" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1046" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="J1046" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="1047" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1047" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="C1047" s="7" t="s">
+        <v>729</v>
+      </c>
+      <c r="D1047" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="E1047" s="7">
+        <v>4</v>
+      </c>
+      <c r="F1047" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1047" s="7"/>
+      <c r="H1047" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1047" s="7"/>
+      <c r="J1047" s="7"/>
+    </row>
+    <row r="1048" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1048" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="C1048" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1048" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1048" s="7">
+        <v>5</v>
+      </c>
+      <c r="F1048" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1048" s="7"/>
+      <c r="H1048" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1048" s="7"/>
+      <c r="J1048" s="7"/>
+    </row>
+    <row r="1049" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1049" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="C1049" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1049" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1049" s="7">
+        <v>6</v>
+      </c>
+      <c r="F1049" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1049" s="7">
+        <v>256</v>
+      </c>
+      <c r="H1049" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1049" s="7"/>
+      <c r="J1049" s="7"/>
+    </row>
+    <row r="1050" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1050" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="C1050" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1050" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1050" s="7">
+        <v>7</v>
+      </c>
+      <c r="F1050" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1050" s="7"/>
+      <c r="H1050" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1050" s="7"/>
+      <c r="J1050" s="7"/>
+    </row>
+    <row r="1051" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1051" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="C1051" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1051" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1051" s="7">
+        <v>8</v>
+      </c>
+      <c r="F1051" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1051" s="7">
+        <v>256</v>
+      </c>
+      <c r="H1051" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1051" s="7"/>
+      <c r="J1051" s="7"/>
+    </row>
+    <row r="1052" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1052" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="C1052" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1052" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1052" s="7">
+        <v>9</v>
+      </c>
+      <c r="F1052" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1052" s="7"/>
+      <c r="H1052" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1052" s="7"/>
+      <c r="J1052" s="7"/>
+    </row>
+    <row r="1053" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1053" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="C1053" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1053" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1053" s="7">
+        <v>10</v>
+      </c>
+      <c r="F1053" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1053" s="7"/>
+      <c r="H1053" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1053" s="7"/>
+      <c r="J1053" s="7"/>
+    </row>
+    <row r="1054" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1054" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="C1054" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1054" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1054" s="7">
+        <v>11</v>
+      </c>
+      <c r="F1054" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1054" s="7"/>
+      <c r="H1054" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1054" s="7"/>
+      <c r="J1054" s="7"/>
+    </row>
   </sheetData>
   <sortState ref="B4:J893">
     <sortCondition ref="B1:B1048576"/>
@@ -24368,8 +28306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A090B9B-1A25-4B8B-85D7-C0AD9CC37900}">
   <dimension ref="B2:L976"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A957" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G983" sqref="G983"/>
+    <sheetView topLeftCell="A976" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J965" sqref="J965:K975"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -54532,6 +58470,9 @@
       <c r="L976" s="2"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="I904:I917">
+    <cfRule type="uniqueValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -54541,8 +58482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{605A82CC-BA50-4093-8100-BE215ACB26A5}">
   <dimension ref="B2:E82"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+    <sheetView topLeftCell="A58" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>